<commit_message>
DB Helper Atualizado #4
Mudanças feitas aí... Também nas tabelas.
Listarei essas mudanças mais a frente, quando forem mais relevantes...
</commit_message>
<xml_diff>
--- a/Tabelas.xlsx
+++ b/Tabelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela 0 - Personagens" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Tabela 2 - Classes" sheetId="2" r:id="rId3"/>
     <sheet name="Tabela 3 - Perícias" sheetId="4" r:id="rId4"/>
     <sheet name="Tabela 4 - Talentos" sheetId="5" r:id="rId5"/>
+    <sheet name="Tabela 5 - Pré-Requisitos" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="321">
   <si>
     <t xml:space="preserve"> Nome (string)</t>
   </si>
@@ -976,6 +977,60 @@
   </si>
   <si>
     <t>Tipo (string)</t>
+  </si>
+  <si>
+    <t>ID do Talento (int)</t>
+  </si>
+  <si>
+    <t>Tipo (String)</t>
+  </si>
+  <si>
+    <t>Especificação (String)</t>
+  </si>
+  <si>
+    <t>Valor (Int)</t>
+  </si>
+  <si>
+    <t>Talento</t>
+  </si>
+  <si>
+    <t>BBA</t>
+  </si>
+  <si>
+    <t>Atributo</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>Pericia</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Tendência</t>
+  </si>
+  <si>
+    <t>LB,NB,CB</t>
+  </si>
+  <si>
+    <t>Ofício</t>
+  </si>
+  <si>
+    <t>Habilidade</t>
+  </si>
+  <si>
+    <t>Forma Selvagem</t>
+  </si>
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Canalizar Energia</t>
+  </si>
+  <si>
+    <t>CB,CN,CM</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1091,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1072,6 +1127,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1389,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -2586,8 +2644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5560,4 +5618,2784 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F212"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>4</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>4</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>5</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>5</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>5</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
+        <v>5</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>6</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>7</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>8</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>10</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>10</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>11</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>11</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>11</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>11</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>12</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>12</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>12</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>12</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>12</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>12</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>13</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>14</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>14</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>14</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>14</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
+        <v>15</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>15</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>15</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>16</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>16</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>17</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>17</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>18</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="D42" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>19</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>20</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>21</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>21</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>21</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>22</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>22</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
+        <v>22</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="14">
+        <v>22</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>23</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>23</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="14">
+        <v>24</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="14">
+        <v>24</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="14">
+        <v>25</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="14">
+        <v>25</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="14">
+        <v>27</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="14">
+        <v>28</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="14">
+        <v>28</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="14">
+        <v>29</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>29</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="14">
+        <v>30</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="14">
+        <v>30</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="14">
+        <v>30</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="14">
+        <v>30</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>31</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>31</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="14">
+        <v>32</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="14">
+        <v>33</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14">
+        <v>34</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="14">
+        <v>34</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="14">
+        <v>35</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D73" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="14">
+        <v>35</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="14">
+        <v>36</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="14">
+        <v>37</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <v>37</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="14">
+        <v>39</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D78" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="14">
+        <v>39</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="14">
+        <v>40</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D80" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="14">
+        <v>41</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D81" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="14">
+        <v>41</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="14">
+        <v>42</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="14">
+        <v>42</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="14">
+        <v>42</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D85" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="14">
+        <v>43</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="14">
+        <v>43</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="14">
+        <v>45</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="14">
+        <v>45</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="14">
+        <v>45</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="14">
+        <v>45</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="14">
+        <v>45</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D92" s="14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="14">
+        <v>46</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D93" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="14">
+        <v>46</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="14">
+        <v>46</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="14">
+        <v>47</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D96" s="14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="14">
+        <v>47</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D97" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="14">
+        <v>47</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="14">
+        <v>47</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="14">
+        <v>47</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="14">
+        <v>47</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="14">
+        <v>48</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D102" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="14">
+        <v>48</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="14">
+        <v>49</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D104" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="14">
+        <v>49</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="14">
+        <v>49</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="14">
+        <v>50</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D107" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="14">
+        <v>50</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="14">
+        <v>51</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D109" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="14">
+        <v>51</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D110" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="14">
+        <v>51</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="14">
+        <v>51</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="14">
+        <v>52</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="14">
+        <v>52</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D114" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="14">
+        <v>54</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D115" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="14">
+        <v>56</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D116" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="14">
+        <v>56</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="14">
+        <v>58</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D118" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="14">
+        <v>58</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C119" s="14"/>
+      <c r="D119" s="14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>58</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>58</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>58</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>59</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>60</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>60</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D125" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>61</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D126" s="14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>61</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>61</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>61</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>62</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>63</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C131" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D131" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>63</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C132" s="14"/>
+      <c r="D132" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>63</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C133" s="14"/>
+      <c r="D133" s="14">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="14">
+        <v>63</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C134" s="14"/>
+      <c r="D134" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>64</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D135" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>64</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" s="14"/>
+      <c r="D136" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>65</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C137" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D137" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>66</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D138" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>66</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C139" s="14"/>
+      <c r="D139" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>67</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D140" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>67</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C141" s="14"/>
+      <c r="D141" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>67</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C142" s="14"/>
+      <c r="D142" s="14">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>67</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C143" s="14"/>
+      <c r="D143" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="14">
+        <v>69</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C144" s="14"/>
+      <c r="D144" s="14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="14">
+        <v>70</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C145" s="14"/>
+      <c r="D145" s="14">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="14">
+        <v>72</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C146" s="14"/>
+      <c r="D146" s="14">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="14">
+        <v>73</v>
+      </c>
+      <c r="B147" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>73</v>
+      </c>
+      <c r="B148" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C148" s="14"/>
+      <c r="D148" s="14">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>75</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C149" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D149" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>75</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D150" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>77</v>
+      </c>
+      <c r="B151" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C151" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D151" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>80</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C152" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D152" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>85</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C153" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="D153" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>85</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C154" s="14"/>
+      <c r="D154" s="14">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>90</v>
+      </c>
+      <c r="B155" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C155" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D155" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>90</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C156" s="14"/>
+      <c r="D156" s="14">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>92</v>
+      </c>
+      <c r="B157" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C157" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D157" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>93</v>
+      </c>
+      <c r="B158" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C158" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D158" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>93</v>
+      </c>
+      <c r="B159" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C159" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D159" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>94</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C160" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="D160" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>97</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C161" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D161" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>101</v>
+      </c>
+      <c r="B162" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C162" s="14"/>
+      <c r="D162" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>102</v>
+      </c>
+      <c r="B163" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C163" s="14"/>
+      <c r="D163" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>103</v>
+      </c>
+      <c r="B164" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C164" s="14"/>
+      <c r="D164" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>107</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C165" s="14"/>
+      <c r="D165" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>108</v>
+      </c>
+      <c r="B166" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C166" s="14"/>
+      <c r="D166" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>109</v>
+      </c>
+      <c r="B167" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C167" s="14"/>
+      <c r="D167" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>112</v>
+      </c>
+      <c r="B168" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C168" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D168" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>112</v>
+      </c>
+      <c r="B169" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C169" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D169" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>113</v>
+      </c>
+      <c r="B170" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C170" s="14"/>
+      <c r="D170" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>114</v>
+      </c>
+      <c r="B171" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C171" s="14"/>
+      <c r="D171" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>116</v>
+      </c>
+      <c r="B172" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C172" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D172" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>116</v>
+      </c>
+      <c r="B173" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C173" s="14"/>
+      <c r="D173" s="14">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>116</v>
+      </c>
+      <c r="B174" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C174" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D174" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>117</v>
+      </c>
+      <c r="B175" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C175" s="14"/>
+      <c r="D175" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>120</v>
+      </c>
+      <c r="B176" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="C176" s="14"/>
+      <c r="D176" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>121</v>
+      </c>
+      <c r="B177" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C177" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D177" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>122</v>
+      </c>
+      <c r="B178" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C178" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D178" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" s="14">
+        <v>122</v>
+      </c>
+      <c r="B179" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C179" s="14"/>
+      <c r="D179" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>124</v>
+      </c>
+      <c r="B180" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C180" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D180" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>126</v>
+      </c>
+      <c r="B181" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C181" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D181" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>127</v>
+      </c>
+      <c r="B182" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C182" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D182" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>128</v>
+      </c>
+      <c r="B183" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C183" s="14"/>
+      <c r="D183" s="14">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>129</v>
+      </c>
+      <c r="B184" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C184" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D184" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>131</v>
+      </c>
+      <c r="B185" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C185" s="14"/>
+      <c r="D185" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>134</v>
+      </c>
+      <c r="B186" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C186" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D186" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>138</v>
+      </c>
+      <c r="B187" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C187" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D187" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>139</v>
+      </c>
+      <c r="B188" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C188" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D188" s="14">
+        <v>0</v>
+      </c>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>140</v>
+      </c>
+      <c r="B189" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C189" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D189" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>141</v>
+      </c>
+      <c r="B190" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C190" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D190" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>142</v>
+      </c>
+      <c r="B191" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C191" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D191" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>143</v>
+      </c>
+      <c r="B192" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C192" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D192" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>144</v>
+      </c>
+      <c r="B193" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C193" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D193" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>145</v>
+      </c>
+      <c r="B194" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C194" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D194" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>146</v>
+      </c>
+      <c r="B195" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C195" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D195" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>147</v>
+      </c>
+      <c r="B196" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C196" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D196" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>148</v>
+      </c>
+      <c r="B197" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C197" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D197" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>149</v>
+      </c>
+      <c r="B198" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C198" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D198" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>150</v>
+      </c>
+      <c r="B199" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C199" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D199" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>151</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C200" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D200" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>152</v>
+      </c>
+      <c r="B201" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C201" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D201" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>153</v>
+      </c>
+      <c r="B202" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C202" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D202" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>154</v>
+      </c>
+      <c r="B203" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C203" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D203" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>155</v>
+      </c>
+      <c r="B204" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C204" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D204" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>156</v>
+      </c>
+      <c r="B205" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C205" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D205" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>157</v>
+      </c>
+      <c r="B206" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C206" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D206" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>158</v>
+      </c>
+      <c r="B207" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C207" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D207" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>159</v>
+      </c>
+      <c r="B208" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C208" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D208" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>162</v>
+      </c>
+      <c r="B209" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C209" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D209" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>164</v>
+      </c>
+      <c r="B210" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C210" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D210" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>166</v>
+      </c>
+      <c r="B211" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C211" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D211" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>167</v>
+      </c>
+      <c r="B212" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C212" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D212" s="14">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DB Helper + Tabelas
Mais métodos criados para exibir as informações na tela. Estou
preocupado com a velocidade de execução; eu li que acessar o banco de
dados é algo que exige bastante memória, e eu preciso fazer isso muitas
vezes.
Ah... Tem como me colocar um botão de testes? Pra eu poder ver se está
funcionando, quando for fazer os testes.
</commit_message>
<xml_diff>
--- a/Tabelas.xlsx
+++ b/Tabelas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela 0 - Personagens" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Tabela 3 - Perícias" sheetId="4" r:id="rId4"/>
     <sheet name="Tabela 4 - Talentos" sheetId="5" r:id="rId5"/>
     <sheet name="Tabela 5 - Pré-Requisitos" sheetId="6" r:id="rId6"/>
+    <sheet name="Tabela 6 - Armas" sheetId="7" r:id="rId7"/>
+    <sheet name="Tabela 7 - Armaduras" sheetId="8" r:id="rId8"/>
+    <sheet name="Tabela 8 - Poder Mágico de Arma" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="428">
   <si>
     <t xml:space="preserve"> Nome (string)</t>
   </si>
@@ -1031,6 +1034,327 @@
   </si>
   <si>
     <t>CB,CN,CM</t>
+  </si>
+  <si>
+    <t>Nome (String)</t>
+  </si>
+  <si>
+    <t>Mão (int)</t>
+  </si>
+  <si>
+    <t>Dificuldade (int)</t>
+  </si>
+  <si>
+    <t>Tipo de Dano (int)</t>
+  </si>
+  <si>
+    <t>Arremesso (int)</t>
+  </si>
+  <si>
+    <t>Alcance (int)</t>
+  </si>
+  <si>
+    <t>Margem de Crítico (int)</t>
+  </si>
+  <si>
+    <t>Multiplicador (int)</t>
+  </si>
+  <si>
+    <t>Acuidade (bool)</t>
+  </si>
+  <si>
+    <t>Haste (bool)</t>
+  </si>
+  <si>
+    <t>Peso (float)</t>
+  </si>
+  <si>
+    <t>Preço (int)</t>
+  </si>
+  <si>
+    <t>Origem (String)</t>
+  </si>
+  <si>
+    <t>Adaga</t>
+  </si>
+  <si>
+    <t>Espada curta</t>
+  </si>
+  <si>
+    <t>Manopla</t>
+  </si>
+  <si>
+    <t>Clava</t>
+  </si>
+  <si>
+    <t>Lança</t>
+  </si>
+  <si>
+    <t>Maça</t>
+  </si>
+  <si>
+    <t>Bordão</t>
+  </si>
+  <si>
+    <t>Pique</t>
+  </si>
+  <si>
+    <t>Tacape</t>
+  </si>
+  <si>
+    <t>Arco curto</t>
+  </si>
+  <si>
+    <t>Besta leve</t>
+  </si>
+  <si>
+    <t>Funda</t>
+  </si>
+  <si>
+    <t>Machadinha</t>
+  </si>
+  <si>
+    <t>Martelo</t>
+  </si>
+  <si>
+    <t>Cimitarra</t>
+  </si>
+  <si>
+    <t>Espada longa</t>
+  </si>
+  <si>
+    <t>Florete</t>
+  </si>
+  <si>
+    <t>Machado de batalha</t>
+  </si>
+  <si>
+    <t>Mangual</t>
+  </si>
+  <si>
+    <t>Martelo de guerra</t>
+  </si>
+  <si>
+    <t>Picareta</t>
+  </si>
+  <si>
+    <t>Tridente</t>
+  </si>
+  <si>
+    <t>Alabarda</t>
+  </si>
+  <si>
+    <t>Alfange</t>
+  </si>
+  <si>
+    <t>Espada grande</t>
+  </si>
+  <si>
+    <t>Foice</t>
+  </si>
+  <si>
+    <t>Lança montada</t>
+  </si>
+  <si>
+    <t>Machado grande</t>
+  </si>
+  <si>
+    <t>Arco composto</t>
+  </si>
+  <si>
+    <t>Arco longo</t>
+  </si>
+  <si>
+    <t>Besta pesada</t>
+  </si>
+  <si>
+    <t>Nunchaku</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>Wakizashi</t>
+  </si>
+  <si>
+    <t>Chicote</t>
+  </si>
+  <si>
+    <t>Espada bastarda</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
+  <si>
+    <t>Machado anão</t>
+  </si>
+  <si>
+    <t>Sabre serrilhado</t>
+  </si>
+  <si>
+    <t>Corrente com cravos</t>
+  </si>
+  <si>
+    <t>Espada de duas lâminas</t>
+  </si>
+  <si>
+    <t>Espada táurica</t>
+  </si>
+  <si>
+    <t>Marreta estilhaçadora</t>
+  </si>
+  <si>
+    <t>Mosquete</t>
+  </si>
+  <si>
+    <t>Pistola</t>
+  </si>
+  <si>
+    <t>Tai-tai</t>
+  </si>
+  <si>
+    <t>Peso (int)</t>
+  </si>
+  <si>
+    <t>Bonus na CA (int)</t>
+  </si>
+  <si>
+    <t>Bonus Max Des (int)</t>
+  </si>
+  <si>
+    <t>Penalidade de Armadura (int)</t>
+  </si>
+  <si>
+    <t>Armadura acolchoada</t>
+  </si>
+  <si>
+    <t>Corselete de couro</t>
+  </si>
+  <si>
+    <t>Couro batido</t>
+  </si>
+  <si>
+    <t>Camisa de cota de malha</t>
+  </si>
+  <si>
+    <t>Gibão de peles</t>
+  </si>
+  <si>
+    <t>Brunea</t>
+  </si>
+  <si>
+    <t>Cota de malha</t>
+  </si>
+  <si>
+    <t>Couraça</t>
+  </si>
+  <si>
+    <t>Cota de talas</t>
+  </si>
+  <si>
+    <t>Loriga segmentada</t>
+  </si>
+  <si>
+    <t>Meia armadura</t>
+  </si>
+  <si>
+    <t>Armadura completa</t>
+  </si>
+  <si>
+    <t>Afiada</t>
+  </si>
+  <si>
+    <t>Antianimais</t>
+  </si>
+  <si>
+    <t>Anticonstrutos</t>
+  </si>
+  <si>
+    <t>Antiespíritos</t>
+  </si>
+  <si>
+    <t>Antihumanoides</t>
+  </si>
+  <si>
+    <t>Antimonstros</t>
+  </si>
+  <si>
+    <t>Antimortos-vivos</t>
+  </si>
+  <si>
+    <t>Armazenar Magia</t>
+  </si>
+  <si>
+    <t>Arremesso</t>
+  </si>
+  <si>
+    <t>Congelante</t>
+  </si>
+  <si>
+    <t>Defensor</t>
+  </si>
+  <si>
+    <t>Dissonante</t>
+  </si>
+  <si>
+    <t>Elétrica</t>
+  </si>
+  <si>
+    <t>Flamejante</t>
+  </si>
+  <si>
+    <t>Misericórdia</t>
+  </si>
+  <si>
+    <t>Toque espectral</t>
+  </si>
+  <si>
+    <t>Trespassar aprimorado</t>
+  </si>
+  <si>
+    <t>Trovejante</t>
+  </si>
+  <si>
+    <t>Anárquica</t>
+  </si>
+  <si>
+    <t>Axiomática</t>
+  </si>
+  <si>
+    <t>Explosão congelante</t>
+  </si>
+  <si>
+    <t>Explosão elétrica</t>
+  </si>
+  <si>
+    <t>Explosão flamejante</t>
+  </si>
+  <si>
+    <t>Profana</t>
+  </si>
+  <si>
+    <t>Rompimento</t>
+  </si>
+  <si>
+    <t>Sagrada</t>
+  </si>
+  <si>
+    <t>Sangramento</t>
+  </si>
+  <si>
+    <t>Dançarina</t>
+  </si>
+  <si>
+    <t>Energia brilhante</t>
+  </si>
+  <si>
+    <t>Velocidade</t>
+  </si>
+  <si>
+    <t>Vorpal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Usabilidade (int)</t>
   </si>
 </sst>
 </file>
@@ -5624,7 +5948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
@@ -8398,4 +8722,2723 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1.5</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B6" s="12">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>341</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>35</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0.25</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>15</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>349</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>15</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>350</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>20</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>351</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>10</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>352</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>2.5</v>
+      </c>
+      <c r="L20">
+        <v>8</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>353</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>2.5</v>
+      </c>
+      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>354</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>355</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>15</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>356</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>10</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>75</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>358</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>50</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>359</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="L27">
+        <v>18</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <v>10</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>361</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>6</v>
+      </c>
+      <c r="L29">
+        <v>20</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>362</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>75</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>363</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>24</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>1.5</v>
+      </c>
+      <c r="L31">
+        <v>100</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>364</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>27</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>50</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>365</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>366</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0.5</v>
+      </c>
+      <c r="L34">
+        <v>5</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>367</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>350</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>368</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>369</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>35</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>370</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>3</v>
+      </c>
+      <c r="L38">
+        <v>100</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>371</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <v>30</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>372</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>500</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>373</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>5</v>
+      </c>
+      <c r="L41">
+        <v>25</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>374</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>5</v>
+      </c>
+      <c r="L42">
+        <v>100</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>375</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>7.5</v>
+      </c>
+      <c r="L43">
+        <v>50</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>376</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>7</v>
+      </c>
+      <c r="L44">
+        <v>50</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>377</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>45</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>5</v>
+      </c>
+      <c r="L45">
+        <v>500</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>378</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>15</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1.5</v>
+      </c>
+      <c r="L46">
+        <v>250</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>379</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>24</v>
+      </c>
+      <c r="G47" s="12">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>40</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="10"/>
+    </row>
+    <row r="49" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K49" s="12"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="10"/>
+    </row>
+    <row r="51" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M52" s="10"/>
+    </row>
+    <row r="53" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M53" s="10"/>
+    </row>
+    <row r="54" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M54" s="10"/>
+    </row>
+    <row r="55" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="M55" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>387</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>200</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>250</v>
+      </c>
+      <c r="G11">
+        <v>17</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>394</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>600</v>
+      </c>
+      <c r="G12">
+        <v>22</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>395</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>1500</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>401</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>404</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>405</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>406</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>407</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>409</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>411</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>412</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>413</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>414</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>415</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>416</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>417</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>418</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>419</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>420</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>421</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>422</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>423</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>424</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>425</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>426</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>